<commit_message>
added several new models
</commit_message>
<xml_diff>
--- a/DDOG.xlsx
+++ b/DDOG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC6A63E-DE74-4A6C-9531-289905C4B407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA743D8-00FC-4620-BF9B-FAF70F861E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18690" yWindow="540" windowWidth="18375" windowHeight="19260" activeTab="1" xr2:uid="{3FD86B5C-07F1-42A4-9D66-8FB9C4BAF175}"/>
+    <workbookView xWindow="-42450" yWindow="915" windowWidth="38700" windowHeight="15345" xr2:uid="{3FD86B5C-07F1-42A4-9D66-8FB9C4BAF175}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3BD0B1-E685-4627-8A01-75A3D2BDF860}">
   <dimension ref="N2:P7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -821,11 +821,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB5D0F6-F818-4D6B-9D91-E5CB5E0CBE0F}">
   <dimension ref="A1:AD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="K30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S21" sqref="S21"/>
+      <selection pane="bottomRight" activeCell="R54" sqref="R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1097,35 +1097,35 @@
         <v>324.21299999999997</v>
       </c>
       <c r="M8" s="6">
-        <f>+M6-M7</f>
+        <f t="shared" ref="M8:T8" si="2">+M6-M7</f>
         <v>342.93400000000003</v>
       </c>
       <c r="N8" s="6">
-        <f>+N6-N7</f>
+        <f t="shared" si="2"/>
         <v>372.642</v>
       </c>
       <c r="O8" s="6">
-        <f>+O6-O7</f>
+        <f t="shared" si="2"/>
         <v>381.8</v>
       </c>
       <c r="P8" s="6">
-        <f>+P6-P7</f>
+        <f t="shared" si="2"/>
         <v>407.61399999999998</v>
       </c>
       <c r="Q8" s="6">
-        <f>+Q6-Q7</f>
+        <f t="shared" si="2"/>
         <v>444.21699999999993</v>
       </c>
       <c r="R8" s="6">
-        <f>+R6-R7</f>
+        <f t="shared" si="2"/>
         <v>484.82</v>
       </c>
       <c r="S8" s="6">
-        <f>+S6-S7</f>
+        <f t="shared" si="2"/>
         <v>501.15500000000003</v>
       </c>
       <c r="T8" s="6">
-        <f>+T6-T7</f>
+        <f t="shared" si="2"/>
         <v>521.78</v>
       </c>
       <c r="U8" s="6"/>
@@ -1313,67 +1313,67 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
-        <f t="shared" ref="E12:L12" si="2">SUM(E9:E11)</f>
+        <f t="shared" ref="E12:L12" si="3">SUM(E9:E11)</f>
         <v>129.958</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>145.613</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>164.71299999999999</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>186.33699999999999</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>212.05100000000002</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>250.59399999999999</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>278.154</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>327.35199999999998</v>
       </c>
       <c r="M12" s="6">
-        <f>+M11+M10+M9</f>
+        <f t="shared" ref="M12:T12" si="4">+M11+M10+M9</f>
         <v>374.27600000000001</v>
       </c>
       <c r="N12" s="6">
-        <f>+N11+N10+N9</f>
+        <f t="shared" si="4"/>
         <v>407.27</v>
       </c>
       <c r="O12" s="6">
-        <f>+O11+O10+O9</f>
+        <f t="shared" si="4"/>
         <v>416.77</v>
       </c>
       <c r="P12" s="6">
-        <f>+P11+P10+P9</f>
+        <f t="shared" si="4"/>
         <v>429.62</v>
       </c>
       <c r="Q12" s="6">
-        <f>+Q11+Q10+Q9</f>
+        <f t="shared" si="4"/>
         <v>448.447</v>
       </c>
       <c r="R12" s="6">
-        <f>+R11+R10+R9</f>
+        <f t="shared" si="4"/>
         <v>457.07799999999997</v>
       </c>
       <c r="S12" s="6">
-        <f>+S11+S10+S9</f>
+        <f t="shared" si="4"/>
         <v>489.15899999999999</v>
       </c>
       <c r="T12" s="6">
-        <f>+T11+T10+T9</f>
+        <f t="shared" si="4"/>
         <v>509.16199999999998</v>
       </c>
       <c r="U12" s="6"/>
@@ -1387,67 +1387,67 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
-        <f t="shared" ref="E13:L13" si="3">E8-E12</f>
+        <f t="shared" ref="E13:L13" si="5">E8-E12</f>
         <v>-9.2669999999999959</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-8.9379999999999882</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-12.829999999999984</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-9.8859999999999673</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-4.8950000000000102</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.4549999999999841</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10.413999999999987</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-3.13900000000001</v>
       </c>
       <c r="M13" s="6">
-        <f>+M8-M12</f>
+        <f t="shared" ref="M13:T13" si="6">+M8-M12</f>
         <v>-31.341999999999985</v>
       </c>
       <c r="N13" s="6">
-        <f>+N8-N12</f>
+        <f t="shared" si="6"/>
         <v>-34.627999999999986</v>
       </c>
       <c r="O13" s="6">
-        <f>+O8-O12</f>
+        <f t="shared" si="6"/>
         <v>-34.96999999999997</v>
       </c>
       <c r="P13" s="6">
-        <f>+P8-P12</f>
+        <f t="shared" si="6"/>
         <v>-22.006000000000029</v>
       </c>
       <c r="Q13" s="6">
-        <f>+Q8-Q12</f>
+        <f t="shared" si="6"/>
         <v>-4.230000000000075</v>
       </c>
       <c r="R13" s="6">
-        <f>+R8-R12</f>
+        <f t="shared" si="6"/>
         <v>27.742000000000019</v>
       </c>
       <c r="S13" s="6">
-        <f>+S8-S12</f>
+        <f t="shared" si="6"/>
         <v>11.996000000000038</v>
       </c>
       <c r="T13" s="6">
-        <f>+T8-T12</f>
+        <f t="shared" si="6"/>
         <v>12.617999999999995</v>
       </c>
       <c r="U13" s="6"/>
@@ -1532,67 +1532,67 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
-        <f t="shared" ref="E15:L15" si="4">+E13+E14</f>
+        <f t="shared" ref="E15:L15" si="7">+E13+E14</f>
         <v>-14.554999999999996</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-15.166999999999987</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-12.528999999999986</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-9.6579999999999675</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-4.7670000000000101</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.531999999999984</v>
       </c>
       <c r="K15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>10.853999999999989</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.1000000000010779E-2</v>
       </c>
       <c r="M15" s="6">
-        <f>+M13+M14</f>
+        <f t="shared" ref="M15:T15" si="8">+M13+M14</f>
         <v>-23.058999999999983</v>
       </c>
       <c r="N15" s="6">
-        <f>+N13+N14</f>
+        <f t="shared" si="8"/>
         <v>-25.853999999999985</v>
       </c>
       <c r="O15" s="6">
-        <f>+O13+O14</f>
+        <f t="shared" si="8"/>
         <v>-20.423999999999971</v>
       </c>
       <c r="P15" s="6">
-        <f>+P13+P14</f>
+        <f t="shared" si="8"/>
         <v>-0.90800000000002967</v>
       </c>
       <c r="Q15" s="6">
-        <f>+Q13+Q14</f>
+        <f t="shared" si="8"/>
         <v>24.299999999999923</v>
       </c>
       <c r="R15" s="6">
-        <f>+R13+R14</f>
+        <f t="shared" si="8"/>
         <v>57.267000000000017</v>
       </c>
       <c r="S15" s="6">
-        <f>+S13+S14</f>
+        <f t="shared" si="8"/>
         <v>46.185000000000038</v>
       </c>
       <c r="T15" s="6">
-        <f>+T13+T14</f>
+        <f t="shared" si="8"/>
         <v>47.792999999999999</v>
       </c>
       <c r="U15" s="6"/>
@@ -1664,67 +1664,67 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
-        <f t="shared" ref="E17:L17" si="5">+E15-E16</f>
+        <f t="shared" ref="E17:L17" si="9">+E15-E16</f>
         <v>-15.149999999999997</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-16.159999999999986</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-11.989999999999986</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-6.6979999999999675</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-4.0500000000000105</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7.1689999999999845</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9.7379999999999889</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-4.8790000000000111</v>
       </c>
       <c r="M17" s="6">
-        <f>+M15-M16</f>
+        <f t="shared" ref="M17:T17" si="10">+M15-M16</f>
         <v>-25.984999999999985</v>
       </c>
       <c r="N17" s="6">
-        <f>+N15-N16</f>
+        <f t="shared" si="10"/>
         <v>-29.033999999999985</v>
       </c>
       <c r="O17" s="6">
-        <f>+O15-O16</f>
+        <f t="shared" si="10"/>
         <v>-24.08599999999997</v>
       </c>
       <c r="P17" s="6">
-        <f>+P15-P16</f>
+        <f t="shared" si="10"/>
         <v>-3.9690000000000296</v>
       </c>
       <c r="Q17" s="6">
-        <f>+Q15-Q16</f>
+        <f t="shared" si="10"/>
         <v>22.629999999999924</v>
       </c>
       <c r="R17" s="6">
-        <f>+R15-R16</f>
+        <f t="shared" si="10"/>
         <v>53.993000000000016</v>
       </c>
       <c r="S17" s="6">
-        <f>+S15-S16</f>
+        <f t="shared" si="10"/>
         <v>42.631000000000036</v>
       </c>
       <c r="T17" s="6">
-        <f>+T15-T16</f>
+        <f t="shared" si="10"/>
         <v>43.823999999999998</v>
       </c>
       <c r="U17" s="6"/>
@@ -1738,67 +1738,67 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7">
-        <f t="shared" ref="E18:L18" si="6">+E17/E19</f>
+        <f t="shared" ref="E18:L18" si="11">+E17/E19</f>
         <v>-5.0073705850856368E-2</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-5.3147929500060795E-2</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-3.9178653352241861E-2</v>
       </c>
       <c r="H18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-2.1745411809011676E-2</v>
       </c>
       <c r="I18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-1.3054114947122809E-2</v>
       </c>
       <c r="J18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2.0727021455604115E-2</v>
       </c>
       <c r="K18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2.8171540321927365E-2</v>
       </c>
       <c r="L18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-1.5498975523753589E-2</v>
       </c>
       <c r="M18" s="7">
-        <f>+M17/M19</f>
+        <f t="shared" ref="M18:T18" si="12">+M17/M19</f>
         <v>-8.223361498781602E-2</v>
       </c>
       <c r="N18" s="7">
-        <f>+N17/N19</f>
+        <f t="shared" si="12"/>
         <v>-9.1489468974122995E-2</v>
       </c>
       <c r="O18" s="7">
-        <f>+O17/O19</f>
+        <f t="shared" si="12"/>
         <v>-7.5437068960117162E-2</v>
       </c>
       <c r="P18" s="7">
-        <f>+P17/P19</f>
+        <f t="shared" si="12"/>
         <v>-1.2317862296913644E-2</v>
       </c>
       <c r="Q18" s="7">
-        <f>+Q17/Q19</f>
+        <f t="shared" si="12"/>
         <v>6.4416226171262123E-2</v>
       </c>
       <c r="R18" s="7">
-        <f>+R17/R19</f>
+        <f t="shared" si="12"/>
         <v>0.15299498168072614</v>
       </c>
       <c r="S18" s="7">
-        <f>+S17/S19</f>
+        <f t="shared" si="12"/>
         <v>0.11975706432121007</v>
       </c>
       <c r="T18" s="7">
-        <f>+T17/T19</f>
+        <f t="shared" si="12"/>
         <v>0.12284577002859225</v>
       </c>
       <c r="U18" s="7"/>
@@ -1874,47 +1874,47 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="10">
-        <f t="shared" ref="I21:K21" si="7">+I6/E6-1</f>
+        <f t="shared" ref="I21:K21" si="13">+I6/E6-1</f>
         <v>0.74875060610958455</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.83741431074009598</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.82841515192723181</v>
       </c>
       <c r="L21" s="10">
-        <f>+L6/H6-1</f>
+        <f t="shared" ref="L21:T21" si="14">+L6/H6-1</f>
         <v>0.73898411040081502</v>
       </c>
       <c r="M21" s="10">
-        <f>+M6/I6-1</f>
+        <f t="shared" si="14"/>
         <v>0.61387196474520134</v>
       </c>
       <c r="N21" s="10">
-        <f>+N6/J6-1</f>
+        <f t="shared" si="14"/>
         <v>0.43900023911857233</v>
       </c>
       <c r="O21" s="10">
-        <f>+O6/K6-1</f>
+        <f t="shared" si="14"/>
         <v>0.32692614935404807</v>
       </c>
       <c r="P21" s="10">
-        <f>+P6/L6-1</f>
+        <f t="shared" si="14"/>
         <v>0.25440121338067367</v>
       </c>
       <c r="Q21" s="10">
-        <f>+Q6/M6-1</f>
+        <f t="shared" si="14"/>
         <v>0.25428318134024219</v>
       </c>
       <c r="R21" s="10">
-        <f>+R6/N6-1</f>
+        <f t="shared" si="14"/>
         <v>0.25617864545940661</v>
       </c>
       <c r="S21" s="10">
-        <f>+S6/O6-1</f>
+        <f t="shared" si="14"/>
         <v>0.26891267432542976</v>
       </c>
       <c r="T21" s="10">
@@ -1930,31 +1930,31 @@
         <v>46</v>
       </c>
       <c r="E22" s="12">
-        <f t="shared" ref="E22:H22" si="8">+E8/E6</f>
+        <f t="shared" ref="E22:H22" si="15">+E8/E6</f>
         <v>0.78028770001616288</v>
       </c>
       <c r="F22" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>0.76986554460911061</v>
       </c>
       <c r="G22" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>0.7649648197674126</v>
       </c>
       <c r="H22" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>0.75552025485015994</v>
       </c>
       <c r="I22" s="12">
-        <f t="shared" ref="I22:K22" si="9">+I8/I6</f>
+        <f t="shared" ref="I22:K22" si="16">+I8/I6</f>
         <v>0.76586022300434775</v>
       </c>
       <c r="J22" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>0.79414649997854059</v>
       </c>
       <c r="K22" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>0.79488747486433631</v>
       </c>
       <c r="L22" s="12">
@@ -1962,35 +1962,35 @@
         <v>0.79828284967178642</v>
       </c>
       <c r="M22" s="12">
-        <f t="shared" ref="M22:P22" si="10">+M8/M6</f>
+        <f t="shared" ref="M22:P22" si="17">+M8/M6</f>
         <v>0.78558551129009724</v>
       </c>
       <c r="N22" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.79387045988593929</v>
       </c>
       <c r="O22" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.79258647247121738</v>
       </c>
       <c r="P22" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.80009029168138812</v>
       </c>
       <c r="Q22" s="12">
-        <f t="shared" ref="Q22:R22" si="11">+Q8/Q6</f>
+        <f t="shared" ref="Q22:R22" si="18">+Q8/Q6</f>
         <v>0.81130190526285029</v>
       </c>
       <c r="R22" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>0.82221796356815668</v>
       </c>
       <c r="S22" s="12">
-        <f t="shared" ref="S22:T22" si="12">+S8/S6</f>
+        <f t="shared" ref="S22:T22" si="19">+S8/S6</f>
         <v>0.81988145661452783</v>
       </c>
       <c r="T22" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>0.80861146883751056</v>
       </c>
       <c r="U22" s="12"/>
@@ -2961,13 +2961,18 @@
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
-      <c r="Q54" s="6"/>
+      <c r="Q54" s="6">
+        <v>439.72800000000001</v>
+      </c>
       <c r="R54" s="6"/>
       <c r="S54" s="6">
         <f>SUM(S44:S53)</f>
         <v>212.26999999999998</v>
       </c>
-      <c r="T54" s="6"/>
+      <c r="T54" s="6">
+        <f>376-S54</f>
+        <v>163.73000000000002</v>
+      </c>
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
       <c r="W54" s="6"/>

</xml_diff>